<commit_message>
Fixed two csv files and updated querys
</commit_message>
<xml_diff>
--- a/excel documents/competition_results.xlsx
+++ b/excel documents/competition_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\github\1dv503\database_assignment3\excel documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E1064F-CBEB-48B1-BCE8-10CA13707655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E97E6F-D0BF-4776-A0F2-C2DE7A62D83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="9465" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5775" yWindow="3705" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Slottsskogen open</t>
   </si>
   <si>
-    <t>slottsskogen</t>
-  </si>
-  <si>
     <t>pure</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>gauntlet</t>
+  </si>
+  <si>
+    <t>Teleborgs discgolfbana</t>
   </si>
 </sst>
 </file>
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
         <v>2019</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -456,10 +456,10 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>2019</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -482,10 +482,10 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>2019</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -508,10 +508,10 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
         <v>2019</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -534,10 +534,10 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>2019</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -560,10 +560,10 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
         <v>2019</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -586,10 +586,10 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
         <v>2019</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -612,10 +612,10 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>2019</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -638,10 +638,10 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>2019</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -664,10 +664,10 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>2019</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -690,10 +690,10 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
         <v>2019</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -716,10 +716,10 @@
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>2019</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -742,10 +742,10 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>2019</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -768,10 +768,10 @@
         <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>2019</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -794,10 +794,10 @@
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>2019</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -820,10 +820,10 @@
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -834,7 +834,7 @@
         <v>2019</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -846,10 +846,10 @@
         <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>2019</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -872,10 +872,10 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -886,7 +886,7 @@
         <v>2019</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -898,10 +898,10 @@
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -912,7 +912,7 @@
         <v>2019</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D20">
         <v>7</v>
@@ -924,10 +924,10 @@
         <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -938,7 +938,7 @@
         <v>2019</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D21">
         <v>7</v>
@@ -950,10 +950,10 @@
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -964,7 +964,7 @@
         <v>2019</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D22">
         <v>7</v>
@@ -976,10 +976,10 @@
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -990,7 +990,7 @@
         <v>2019</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D23">
         <v>8</v>
@@ -1002,10 +1002,10 @@
         <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1016,7 +1016,7 @@
         <v>2019</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D24">
         <v>8</v>
@@ -1028,10 +1028,10 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>2019</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D25">
         <v>8</v>
@@ -1054,10 +1054,10 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1068,7 +1068,7 @@
         <v>2019</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D26">
         <v>9</v>
@@ -1080,10 +1080,10 @@
         <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
         <v>2019</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D27">
         <v>9</v>
@@ -1106,10 +1106,10 @@
         <v>5</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
         <v>2019</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D28">
         <v>9</v>
@@ -1132,10 +1132,10 @@
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1146,7 +1146,7 @@
         <v>2020</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1158,10 +1158,10 @@
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1172,7 +1172,7 @@
         <v>2020</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1184,10 +1184,10 @@
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
         <v>2020</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1210,10 +1210,10 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>2020</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D32">
         <v>4</v>
@@ -1236,10 +1236,10 @@
         <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
         <v>2020</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D33">
         <v>5</v>
@@ -1262,10 +1262,10 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
         <v>2020</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D34">
         <v>6</v>
@@ -1288,10 +1288,10 @@
         <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1302,7 +1302,7 @@
         <v>2020</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D35">
         <v>7</v>
@@ -1314,10 +1314,10 @@
         <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
         <v>2020</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D36">
         <v>8</v>
@@ -1340,10 +1340,10 @@
         <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1354,7 +1354,7 @@
         <v>2020</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D37">
         <v>9</v>
@@ -1366,10 +1366,10 @@
         <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1380,7 +1380,7 @@
         <v>2020</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1392,10 +1392,10 @@
         <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
         <v>2020</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -1418,10 +1418,10 @@
         <v>3</v>
       </c>
       <c r="G39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>2020</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -1444,10 +1444,10 @@
         <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1458,7 +1458,7 @@
         <v>2020</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -1470,10 +1470,10 @@
         <v>5</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1484,7 +1484,7 @@
         <v>2020</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D42">
         <v>5</v>
@@ -1496,10 +1496,10 @@
         <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>2020</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D43">
         <v>6</v>
@@ -1522,10 +1522,10 @@
         <v>5</v>
       </c>
       <c r="G43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1536,7 +1536,7 @@
         <v>2020</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D44">
         <v>7</v>
@@ -1548,10 +1548,10 @@
         <v>4</v>
       </c>
       <c r="G44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>2020</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D45">
         <v>8</v>
@@ -1574,10 +1574,10 @@
         <v>6</v>
       </c>
       <c r="G45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
         <v>2020</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D46">
         <v>9</v>
@@ -1600,10 +1600,10 @@
         <v>6</v>
       </c>
       <c r="G46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>